<commit_message>
Overwrite existing (connection issue)
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SebastianLabuschagne\OneDrive - Larc AI (Pty) Ltd\Documents\CMPG323 Repositories\Connected Office Web Application User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0646ADDA-505B-4D8E-9BDF-E07F1874C7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566F42E8-A59A-4FA6-8A0D-49CEF03EFA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -698,7 +698,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +922,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,7 +1052,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1139,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updateed Read logic (now works)
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SebastianLabuschagne\OneDrive - Larc AI (Pty) Ltd\Documents\CMPG323 Repositories\Connected Office Web Application User Acceptance Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SebastianLabuschagne\source\repos\Project 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566F42E8-A59A-4FA6-8A0D-49CEF03EFA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C808D2F-C558-4631-8CA9-C5F276633EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -1139,7 +1139,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1172,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Created Edit and Delete Flow
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SebastianLabuschagne\source\repos\Project 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C808D2F-C558-4631-8CA9-C5F276633EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8082AEED-1015-4271-8F3D-0736E78D8E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -922,7 +922,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1139,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1172,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Updated results tab post run
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SebastianLabuschagne\source\repos\Project 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91664BD3-7201-4AE5-A368-0281CAE1C74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C5F337-732F-4EA8-8E7C-011F622B711F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1139,7 +1139,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,10 +1178,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1195,10 +1195,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1212,10 +1212,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1229,10 +1229,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,10 +1246,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1263,10 +1263,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1280,10 +1280,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1297,10 +1297,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1314,10 +1314,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1331,10 +1331,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1348,10 +1348,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1365,10 +1365,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1382,10 +1382,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1399,10 +1399,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1484,10 +1484,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1501,10 +1501,10 @@
         <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1518,10 +1518,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1535,10 +1535,10 @@
         <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1552,10 +1552,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>